<commit_message>
edit gender seeder, show list profiles of employee
</commit_message>
<xml_diff>
--- a/db_29_10_2018.xlsx
+++ b/db_29_10_2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="4515" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="4515"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="3" r:id="rId1"/>
@@ -21887,7 +21887,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -21898,9 +21898,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -31103,7 +31103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31398,7 +31398,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31638,7 +31638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>